<commit_message>
WBS file issue number update
</commit_message>
<xml_diff>
--- a/결과물/WBS.xlsx
+++ b/결과물/WBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woo/Desktop/boostcamp_git_exmaple/gitflowex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woo/Desktop/boostcamp_git_exmaple/gitflowex/결과물/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9507570-8183-3847-8877-06BD543C8E07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09095C4-8A2D-FB43-91E1-5072D722FD73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -802,7 +802,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1091,6 +1091,81 @@
     <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1100,21 +1175,6 @@
     <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1122,69 +1182,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1528,7 +1525,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1550,34 +1547,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:105">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="107" t="s">
+      <c r="E1" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="107" t="s">
+      <c r="I1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="107" t="s">
+      <c r="J1" s="97" t="s">
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1690,16 +1687,16 @@
       <c r="DA1" s="14"/>
     </row>
     <row r="2" spans="1:105">
-      <c r="A2" s="123"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
       <c r="L2" s="16">
         <v>43486</v>
       </c>
@@ -1880,17 +1877,17 @@
       <c r="DA2" s="19"/>
     </row>
     <row r="3" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="103">
-        <v>1</v>
+      <c r="D3" s="118">
+        <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>21</v>
@@ -2003,10 +2000,10 @@
       <c r="DA3" s="24"/>
     </row>
     <row r="4" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A4" s="124"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="99"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="119"/>
       <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2114,10 +2111,10 @@
       <c r="DA4" s="24"/>
     </row>
     <row r="5" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A5" s="124"/>
-      <c r="B5" s="126"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="99"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
@@ -2225,10 +2222,10 @@
       <c r="DA5" s="24"/>
     </row>
     <row r="6" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A6" s="124"/>
-      <c r="B6" s="126"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="100"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="120"/>
       <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
@@ -2336,13 +2333,13 @@
       <c r="DA6" s="24"/>
     </row>
     <row r="7" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A7" s="124"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="117" t="s">
+      <c r="A7" s="103"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="103">
-        <v>2</v>
+      <c r="D7" s="118">
+        <v>4</v>
       </c>
       <c r="E7" s="77" t="s">
         <v>26</v>
@@ -2451,10 +2448,10 @@
       <c r="DA7" s="24"/>
     </row>
     <row r="8" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A8" s="124"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="99"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="72" t="s">
         <v>27</v>
       </c>
@@ -2562,10 +2559,10 @@
       <c r="DA8" s="24"/>
     </row>
     <row r="9" spans="1:105" ht="18.5" customHeight="1">
-      <c r="A9" s="124"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="100"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="120"/>
       <c r="E9" s="76" t="s">
         <v>28</v>
       </c>
@@ -2620,13 +2617,13 @@
       <c r="BA9" s="22"/>
     </row>
     <row r="10" spans="1:105">
-      <c r="A10" s="124"/>
-      <c r="B10" s="126"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="60" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="92">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E10" s="74" t="s">
         <v>29</v>
@@ -2682,13 +2679,13 @@
       <c r="BA10" s="22"/>
     </row>
     <row r="11" spans="1:105">
-      <c r="A11" s="124"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="117" t="s">
+      <c r="A11" s="103"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="103">
-        <v>4</v>
+      <c r="D11" s="118">
+        <v>8</v>
       </c>
       <c r="E11" s="77" t="s">
         <v>31</v>
@@ -2745,10 +2742,10 @@
       <c r="BA11" s="22"/>
     </row>
     <row r="12" spans="1:105">
-      <c r="A12" s="124"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="100"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="120"/>
       <c r="E12" s="65" t="s">
         <v>32</v>
       </c>
@@ -2803,13 +2800,13 @@
       <c r="BA12" s="22"/>
     </row>
     <row r="13" spans="1:105">
-      <c r="A13" s="124"/>
-      <c r="B13" s="126"/>
-      <c r="C13" s="117" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="103">
-        <v>5</v>
+      <c r="D13" s="118">
+        <v>9</v>
       </c>
       <c r="E13" s="77" t="s">
         <v>34</v>
@@ -2865,10 +2862,10 @@
       <c r="BA13" s="27"/>
     </row>
     <row r="14" spans="1:105">
-      <c r="A14" s="124"/>
-      <c r="B14" s="126"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="100"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="120"/>
       <c r="E14" s="77" t="s">
         <v>35</v>
       </c>
@@ -2923,13 +2920,13 @@
       <c r="BA14" s="34"/>
     </row>
     <row r="15" spans="1:105" ht="15.5" customHeight="1">
-      <c r="A15" s="124"/>
-      <c r="B15" s="126"/>
-      <c r="C15" s="117" t="s">
+      <c r="A15" s="103"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="103">
-        <v>6</v>
+      <c r="D15" s="118">
+        <v>10</v>
       </c>
       <c r="E15" s="75" t="s">
         <v>37</v>
@@ -2986,10 +2983,10 @@
       <c r="BA15" s="22"/>
     </row>
     <row r="16" spans="1:105">
-      <c r="A16" s="124"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="100"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="120"/>
       <c r="E16" s="76" t="s">
         <v>38</v>
       </c>
@@ -3045,15 +3042,15 @@
       <c r="BA16" s="22"/>
     </row>
     <row r="17" spans="1:53">
-      <c r="A17" s="124"/>
-      <c r="B17" s="113" t="s">
+      <c r="A17" s="103"/>
+      <c r="B17" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="103">
-        <v>7</v>
+      <c r="D17" s="118">
+        <v>11</v>
       </c>
       <c r="E17" s="77" t="s">
         <v>41</v>
@@ -3112,10 +3109,10 @@
       <c r="BA17" s="22"/>
     </row>
     <row r="18" spans="1:53">
-      <c r="A18" s="124"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="99"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="119"/>
       <c r="E18" s="77" t="s">
         <v>42</v>
       </c>
@@ -3170,10 +3167,10 @@
       <c r="BA18" s="22"/>
     </row>
     <row r="19" spans="1:53">
-      <c r="A19" s="124"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="100"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="120"/>
       <c r="E19" s="66" t="s">
         <v>43</v>
       </c>
@@ -3228,13 +3225,13 @@
       <c r="BA19" s="22"/>
     </row>
     <row r="20" spans="1:53">
-      <c r="A20" s="124"/>
-      <c r="B20" s="114"/>
-      <c r="C20" s="113" t="s">
+      <c r="A20" s="103"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="96">
-        <v>8</v>
+      <c r="D20" s="121">
+        <v>12</v>
       </c>
       <c r="E20" s="77" t="s">
         <v>41</v>
@@ -3283,10 +3280,10 @@
       <c r="BA20" s="7"/>
     </row>
     <row r="21" spans="1:53">
-      <c r="A21" s="124"/>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="97"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="122"/>
       <c r="E21" s="77" t="s">
         <v>42</v>
       </c>
@@ -3334,10 +3331,10 @@
       <c r="BA21" s="7"/>
     </row>
     <row r="22" spans="1:53">
-      <c r="A22" s="124"/>
-      <c r="B22" s="115"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="98"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="76" t="s">
         <v>43</v>
       </c>
@@ -3385,15 +3382,15 @@
       <c r="BA22" s="7"/>
     </row>
     <row r="23" spans="1:53">
-      <c r="A23" s="124"/>
-      <c r="B23" s="113" t="s">
+      <c r="A23" s="103"/>
+      <c r="B23" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="103">
-        <v>9</v>
+      <c r="D23" s="118">
+        <v>13</v>
       </c>
       <c r="E23" s="77" t="s">
         <v>46</v>
@@ -3444,10 +3441,10 @@
       <c r="BA23" s="7"/>
     </row>
     <row r="24" spans="1:53">
-      <c r="A24" s="124"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="99"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="119"/>
       <c r="E24" s="61" t="s">
         <v>47</v>
       </c>
@@ -3495,10 +3492,10 @@
       <c r="BA24" s="7"/>
     </row>
     <row r="25" spans="1:53">
-      <c r="A25" s="124"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="100"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="120"/>
       <c r="E25" s="78" t="s">
         <v>48</v>
       </c>
@@ -3546,13 +3543,13 @@
       <c r="BA25" s="7"/>
     </row>
     <row r="26" spans="1:53">
-      <c r="A26" s="124"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="117" t="s">
+      <c r="A26" s="103"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="103">
-        <v>10</v>
+      <c r="D26" s="118">
+        <v>14</v>
       </c>
       <c r="E26" s="73" t="s">
         <v>50</v>
@@ -3601,10 +3598,10 @@
       <c r="BA26" s="7"/>
     </row>
     <row r="27" spans="1:53">
-      <c r="A27" s="124"/>
-      <c r="B27" s="115"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="100"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="120"/>
       <c r="E27" s="76" t="s">
         <v>51</v>
       </c>
@@ -3652,15 +3649,15 @@
       <c r="BA27" s="7"/>
     </row>
     <row r="28" spans="1:53">
-      <c r="A28" s="124"/>
-      <c r="B28" s="113" t="s">
+      <c r="A28" s="103"/>
+      <c r="B28" s="107" t="s">
         <v>56</v>
       </c>
       <c r="C28" s="60" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="92">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E28" s="67" t="s">
         <v>52</v>
@@ -3711,13 +3708,13 @@
       <c r="BA28" s="7"/>
     </row>
     <row r="29" spans="1:53">
-      <c r="A29" s="124"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="117" t="s">
+      <c r="A29" s="103"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="103">
-        <v>12</v>
+      <c r="D29" s="118">
+        <v>16</v>
       </c>
       <c r="E29" s="75" t="s">
         <v>54</v>
@@ -3766,10 +3763,10 @@
       <c r="BA29" s="7"/>
     </row>
     <row r="30" spans="1:53">
-      <c r="A30" s="124"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="118"/>
-      <c r="D30" s="99"/>
+      <c r="A30" s="103"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="119"/>
       <c r="E30" s="77" t="s">
         <v>41</v>
       </c>
@@ -3817,10 +3814,10 @@
       <c r="BA30" s="7"/>
     </row>
     <row r="31" spans="1:53">
-      <c r="A31" s="124"/>
-      <c r="B31" s="115"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="100"/>
+      <c r="A31" s="103"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="120"/>
       <c r="E31" s="76" t="s">
         <v>55</v>
       </c>
@@ -3868,17 +3865,17 @@
       <c r="BA31" s="7"/>
     </row>
     <row r="32" spans="1:53">
-      <c r="A32" s="113" t="s">
+      <c r="A32" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="113" t="s">
+      <c r="B32" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="117" t="s">
+      <c r="C32" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="103">
-        <v>13</v>
+      <c r="D32" s="118">
+        <v>17</v>
       </c>
       <c r="E32" s="58" t="s">
         <v>60</v>
@@ -3929,10 +3926,10 @@
       <c r="BA32" s="7"/>
     </row>
     <row r="33" spans="1:53">
-      <c r="A33" s="114"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="119"/>
-      <c r="D33" s="100"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="120"/>
       <c r="E33" s="76" t="s">
         <v>23</v>
       </c>
@@ -3980,13 +3977,13 @@
       <c r="BA33" s="7"/>
     </row>
     <row r="34" spans="1:53" ht="30">
-      <c r="A34" s="114"/>
-      <c r="B34" s="114"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="108"/>
       <c r="C34" s="60" t="s">
         <v>61</v>
       </c>
       <c r="D34" s="92">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E34" s="71" t="s">
         <v>62</v>
@@ -4035,13 +4032,13 @@
       <c r="BA34" s="7"/>
     </row>
     <row r="35" spans="1:53">
-      <c r="A35" s="114"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="117" t="s">
+      <c r="A35" s="108"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="103">
-        <v>15</v>
+      <c r="D35" s="118">
+        <v>19</v>
       </c>
       <c r="E35" s="68" t="s">
         <v>97</v>
@@ -4090,10 +4087,10 @@
       <c r="BA35" s="7"/>
     </row>
     <row r="36" spans="1:53">
-      <c r="A36" s="114"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="119"/>
-      <c r="D36" s="100"/>
+      <c r="A36" s="108"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="101"/>
+      <c r="D36" s="120"/>
       <c r="E36" s="62" t="s">
         <v>64</v>
       </c>
@@ -4141,13 +4138,13 @@
       <c r="BA36" s="7"/>
     </row>
     <row r="37" spans="1:53">
-      <c r="A37" s="114"/>
-      <c r="B37" s="115"/>
+      <c r="A37" s="108"/>
+      <c r="B37" s="109"/>
       <c r="C37" s="60" t="s">
         <v>65</v>
       </c>
       <c r="D37" s="93">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E37" s="41" t="s">
         <v>66</v>
@@ -4196,15 +4193,15 @@
       <c r="BA37" s="7"/>
     </row>
     <row r="38" spans="1:53">
-      <c r="A38" s="114"/>
-      <c r="B38" s="113" t="s">
+      <c r="A38" s="108"/>
+      <c r="B38" s="107" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="94">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E38" s="69" t="s">
         <v>23</v>
@@ -4253,13 +4250,13 @@
       <c r="BA38" s="7"/>
     </row>
     <row r="39" spans="1:53">
-      <c r="A39" s="114"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="120" t="s">
+      <c r="A39" s="108"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="104">
-        <v>18</v>
+      <c r="D39" s="124">
+        <v>22</v>
       </c>
       <c r="E39" s="57" t="s">
         <v>69</v>
@@ -4308,10 +4305,10 @@
       <c r="BA39" s="7"/>
     </row>
     <row r="40" spans="1:53">
-      <c r="A40" s="114"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="121"/>
-      <c r="D40" s="105"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="125"/>
       <c r="E40" s="77" t="s">
         <v>70</v>
       </c>
@@ -4366,10 +4363,10 @@
       <c r="BA40" s="41"/>
     </row>
     <row r="41" spans="1:53">
-      <c r="A41" s="115"/>
-      <c r="B41" s="115"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="106"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="126"/>
       <c r="E41" s="76" t="s">
         <v>71</v>
       </c>
@@ -4380,19 +4377,61 @@
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="46"/>
+      <c r="S41" s="39"/>
+      <c r="T41" s="39"/>
+      <c r="U41" s="39"/>
+      <c r="V41" s="39"/>
+      <c r="W41" s="39"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="51"/>
+      <c r="Z41" s="38"/>
+      <c r="AA41" s="39"/>
+      <c r="AB41" s="39"/>
+      <c r="AC41" s="39"/>
+      <c r="AD41" s="39"/>
+      <c r="AE41" s="51"/>
+      <c r="AF41" s="52"/>
+      <c r="AG41" s="51"/>
+      <c r="AH41" s="51"/>
+      <c r="AI41" s="51"/>
+      <c r="AJ41" s="39"/>
+      <c r="AK41" s="39"/>
+      <c r="AL41" s="51"/>
+      <c r="AM41" s="51"/>
+      <c r="AN41" s="38"/>
+      <c r="AO41" s="39"/>
+      <c r="AP41" s="39"/>
+      <c r="AQ41" s="39"/>
+      <c r="AR41" s="39"/>
+      <c r="AS41" s="51"/>
+      <c r="AT41" s="52"/>
+      <c r="AU41" s="38"/>
+      <c r="AV41" s="28"/>
+      <c r="AW41" s="39"/>
+      <c r="AX41" s="40"/>
+      <c r="AY41" s="40"/>
+      <c r="AZ41" s="40"/>
+      <c r="BA41" s="41"/>
     </row>
     <row r="42" spans="1:53">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="114" t="s">
+      <c r="B42" s="108" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="60" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="92">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E42" s="74" t="s">
         <v>75</v>
@@ -4406,15 +4445,57 @@
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="46"/>
+      <c r="S42" s="39"/>
+      <c r="T42" s="39"/>
+      <c r="U42" s="39"/>
+      <c r="V42" s="39"/>
+      <c r="W42" s="39"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
+      <c r="Z42" s="38"/>
+      <c r="AA42" s="39"/>
+      <c r="AB42" s="39"/>
+      <c r="AC42" s="39"/>
+      <c r="AD42" s="39"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="52"/>
+      <c r="AG42" s="51"/>
+      <c r="AH42" s="51"/>
+      <c r="AI42" s="51"/>
+      <c r="AJ42" s="39"/>
+      <c r="AK42" s="39"/>
+      <c r="AL42" s="51"/>
+      <c r="AM42" s="51"/>
+      <c r="AN42" s="38"/>
+      <c r="AO42" s="39"/>
+      <c r="AP42" s="39"/>
+      <c r="AQ42" s="39"/>
+      <c r="AR42" s="39"/>
+      <c r="AS42" s="51"/>
+      <c r="AT42" s="52"/>
+      <c r="AU42" s="38"/>
+      <c r="AV42" s="28"/>
+      <c r="AW42" s="39"/>
+      <c r="AX42" s="40"/>
+      <c r="AY42" s="40"/>
+      <c r="AZ42" s="40"/>
+      <c r="BA42" s="41"/>
     </row>
     <row r="43" spans="1:53">
-      <c r="A43" s="114"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114" t="s">
+      <c r="A43" s="108"/>
+      <c r="B43" s="108"/>
+      <c r="C43" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="96">
-        <v>20</v>
+      <c r="D43" s="121">
+        <v>24</v>
       </c>
       <c r="E43" s="75" t="s">
         <v>76</v>
@@ -4426,12 +4507,54 @@
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39"/>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="39"/>
+      <c r="T43" s="39"/>
+      <c r="U43" s="39"/>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="51"/>
+      <c r="Z43" s="38"/>
+      <c r="AA43" s="39"/>
+      <c r="AB43" s="39"/>
+      <c r="AC43" s="39"/>
+      <c r="AD43" s="39"/>
+      <c r="AE43" s="51"/>
+      <c r="AF43" s="52"/>
+      <c r="AG43" s="51"/>
+      <c r="AH43" s="51"/>
+      <c r="AI43" s="51"/>
+      <c r="AJ43" s="39"/>
+      <c r="AK43" s="39"/>
+      <c r="AL43" s="51"/>
+      <c r="AM43" s="51"/>
+      <c r="AN43" s="38"/>
+      <c r="AO43" s="39"/>
+      <c r="AP43" s="39"/>
+      <c r="AQ43" s="39"/>
+      <c r="AR43" s="39"/>
+      <c r="AS43" s="51"/>
+      <c r="AT43" s="52"/>
+      <c r="AU43" s="38"/>
+      <c r="AV43" s="28"/>
+      <c r="AW43" s="39"/>
+      <c r="AX43" s="40"/>
+      <c r="AY43" s="40"/>
+      <c r="AZ43" s="40"/>
+      <c r="BA43" s="41"/>
     </row>
     <row r="44" spans="1:53">
-      <c r="A44" s="115"/>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="98"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="123"/>
       <c r="E44" s="76" t="s">
         <v>77</v>
       </c>
@@ -4442,19 +4565,61 @@
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="46"/>
+      <c r="S44" s="39"/>
+      <c r="T44" s="39"/>
+      <c r="U44" s="39"/>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="51"/>
+      <c r="Z44" s="38"/>
+      <c r="AA44" s="39"/>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="39"/>
+      <c r="AE44" s="51"/>
+      <c r="AF44" s="52"/>
+      <c r="AG44" s="51"/>
+      <c r="AH44" s="51"/>
+      <c r="AI44" s="51"/>
+      <c r="AJ44" s="39"/>
+      <c r="AK44" s="39"/>
+      <c r="AL44" s="51"/>
+      <c r="AM44" s="51"/>
+      <c r="AN44" s="38"/>
+      <c r="AO44" s="39"/>
+      <c r="AP44" s="39"/>
+      <c r="AQ44" s="39"/>
+      <c r="AR44" s="39"/>
+      <c r="AS44" s="51"/>
+      <c r="AT44" s="52"/>
+      <c r="AU44" s="38"/>
+      <c r="AV44" s="28"/>
+      <c r="AW44" s="39"/>
+      <c r="AX44" s="40"/>
+      <c r="AY44" s="40"/>
+      <c r="AZ44" s="40"/>
+      <c r="BA44" s="41"/>
     </row>
     <row r="45" spans="1:53">
-      <c r="A45" s="110" t="s">
+      <c r="A45" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="96">
-        <v>21</v>
+      <c r="D45" s="121">
+        <v>25</v>
       </c>
       <c r="E45" s="75" t="s">
         <v>19</v>
@@ -4466,12 +4631,54 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="39"/>
+      <c r="T45" s="39"/>
+      <c r="U45" s="39"/>
+      <c r="V45" s="39"/>
+      <c r="W45" s="39"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="51"/>
+      <c r="Z45" s="38"/>
+      <c r="AA45" s="39"/>
+      <c r="AB45" s="39"/>
+      <c r="AC45" s="39"/>
+      <c r="AD45" s="39"/>
+      <c r="AE45" s="51"/>
+      <c r="AF45" s="52"/>
+      <c r="AG45" s="51"/>
+      <c r="AH45" s="51"/>
+      <c r="AI45" s="51"/>
+      <c r="AJ45" s="39"/>
+      <c r="AK45" s="39"/>
+      <c r="AL45" s="51"/>
+      <c r="AM45" s="51"/>
+      <c r="AN45" s="38"/>
+      <c r="AO45" s="39"/>
+      <c r="AP45" s="39"/>
+      <c r="AQ45" s="39"/>
+      <c r="AR45" s="39"/>
+      <c r="AS45" s="51"/>
+      <c r="AT45" s="52"/>
+      <c r="AU45" s="38"/>
+      <c r="AV45" s="28"/>
+      <c r="AW45" s="39"/>
+      <c r="AX45" s="40"/>
+      <c r="AY45" s="40"/>
+      <c r="AZ45" s="40"/>
+      <c r="BA45" s="41"/>
     </row>
     <row r="46" spans="1:53">
-      <c r="A46" s="111"/>
-      <c r="B46" s="114"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="97"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="122"/>
       <c r="E46" s="77" t="s">
         <v>81</v>
       </c>
@@ -4482,12 +4689,54 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="45"/>
+      <c r="R46" s="46"/>
+      <c r="S46" s="39"/>
+      <c r="T46" s="39"/>
+      <c r="U46" s="39"/>
+      <c r="V46" s="39"/>
+      <c r="W46" s="39"/>
+      <c r="X46" s="51"/>
+      <c r="Y46" s="51"/>
+      <c r="Z46" s="38"/>
+      <c r="AA46" s="39"/>
+      <c r="AB46" s="39"/>
+      <c r="AC46" s="39"/>
+      <c r="AD46" s="39"/>
+      <c r="AE46" s="51"/>
+      <c r="AF46" s="52"/>
+      <c r="AG46" s="51"/>
+      <c r="AH46" s="51"/>
+      <c r="AI46" s="51"/>
+      <c r="AJ46" s="39"/>
+      <c r="AK46" s="39"/>
+      <c r="AL46" s="51"/>
+      <c r="AM46" s="51"/>
+      <c r="AN46" s="38"/>
+      <c r="AO46" s="39"/>
+      <c r="AP46" s="39"/>
+      <c r="AQ46" s="39"/>
+      <c r="AR46" s="39"/>
+      <c r="AS46" s="51"/>
+      <c r="AT46" s="52"/>
+      <c r="AU46" s="38"/>
+      <c r="AV46" s="28"/>
+      <c r="AW46" s="39"/>
+      <c r="AX46" s="40"/>
+      <c r="AY46" s="40"/>
+      <c r="AZ46" s="40"/>
+      <c r="BA46" s="41"/>
     </row>
     <row r="47" spans="1:53">
-      <c r="A47" s="111"/>
-      <c r="B47" s="114"/>
-      <c r="C47" s="115"/>
-      <c r="D47" s="98"/>
+      <c r="A47" s="116"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="109"/>
+      <c r="D47" s="123"/>
       <c r="E47" s="76" t="s">
         <v>82</v>
       </c>
@@ -4498,15 +4747,57 @@
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="45"/>
+      <c r="R47" s="46"/>
+      <c r="S47" s="39"/>
+      <c r="T47" s="39"/>
+      <c r="U47" s="39"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="51"/>
+      <c r="Z47" s="38"/>
+      <c r="AA47" s="39"/>
+      <c r="AB47" s="39"/>
+      <c r="AC47" s="39"/>
+      <c r="AD47" s="39"/>
+      <c r="AE47" s="51"/>
+      <c r="AF47" s="52"/>
+      <c r="AG47" s="51"/>
+      <c r="AH47" s="51"/>
+      <c r="AI47" s="51"/>
+      <c r="AJ47" s="39"/>
+      <c r="AK47" s="39"/>
+      <c r="AL47" s="51"/>
+      <c r="AM47" s="51"/>
+      <c r="AN47" s="38"/>
+      <c r="AO47" s="39"/>
+      <c r="AP47" s="39"/>
+      <c r="AQ47" s="39"/>
+      <c r="AR47" s="39"/>
+      <c r="AS47" s="51"/>
+      <c r="AT47" s="52"/>
+      <c r="AU47" s="38"/>
+      <c r="AV47" s="28"/>
+      <c r="AW47" s="39"/>
+      <c r="AX47" s="40"/>
+      <c r="AY47" s="40"/>
+      <c r="AZ47" s="40"/>
+      <c r="BA47" s="41"/>
     </row>
     <row r="48" spans="1:53">
-      <c r="A48" s="111"/>
-      <c r="B48" s="114"/>
-      <c r="C48" s="113" t="s">
+      <c r="A48" s="116"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="96">
-        <v>22</v>
+      <c r="D48" s="121">
+        <v>26</v>
       </c>
       <c r="E48" s="75" t="s">
         <v>85</v>
@@ -4518,12 +4809,54 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:49">
-      <c r="A49" s="111"/>
-      <c r="B49" s="115"/>
-      <c r="C49" s="115"/>
-      <c r="D49" s="98"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="46"/>
+      <c r="S48" s="39"/>
+      <c r="T48" s="39"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="39"/>
+      <c r="W48" s="39"/>
+      <c r="X48" s="51"/>
+      <c r="Y48" s="51"/>
+      <c r="Z48" s="38"/>
+      <c r="AA48" s="39"/>
+      <c r="AB48" s="39"/>
+      <c r="AC48" s="39"/>
+      <c r="AD48" s="39"/>
+      <c r="AE48" s="51"/>
+      <c r="AF48" s="52"/>
+      <c r="AG48" s="51"/>
+      <c r="AH48" s="51"/>
+      <c r="AI48" s="51"/>
+      <c r="AJ48" s="39"/>
+      <c r="AK48" s="39"/>
+      <c r="AL48" s="51"/>
+      <c r="AM48" s="51"/>
+      <c r="AN48" s="38"/>
+      <c r="AO48" s="39"/>
+      <c r="AP48" s="39"/>
+      <c r="AQ48" s="39"/>
+      <c r="AR48" s="39"/>
+      <c r="AS48" s="51"/>
+      <c r="AT48" s="52"/>
+      <c r="AU48" s="38"/>
+      <c r="AV48" s="28"/>
+      <c r="AW48" s="39"/>
+      <c r="AX48" s="40"/>
+      <c r="AY48" s="40"/>
+      <c r="AZ48" s="40"/>
+      <c r="BA48" s="41"/>
+    </row>
+    <row r="49" spans="1:53">
+      <c r="A49" s="116"/>
+      <c r="B49" s="109"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="123"/>
       <c r="E49" s="76" t="s">
         <v>84</v>
       </c>
@@ -4534,17 +4867,59 @@
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
-    </row>
-    <row r="50" spans="1:49">
-      <c r="A50" s="111"/>
-      <c r="B50" s="113" t="s">
+      <c r="L49" s="38"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="46"/>
+      <c r="S49" s="39"/>
+      <c r="T49" s="39"/>
+      <c r="U49" s="39"/>
+      <c r="V49" s="39"/>
+      <c r="W49" s="39"/>
+      <c r="X49" s="51"/>
+      <c r="Y49" s="51"/>
+      <c r="Z49" s="38"/>
+      <c r="AA49" s="39"/>
+      <c r="AB49" s="39"/>
+      <c r="AC49" s="39"/>
+      <c r="AD49" s="39"/>
+      <c r="AE49" s="51"/>
+      <c r="AF49" s="52"/>
+      <c r="AG49" s="51"/>
+      <c r="AH49" s="51"/>
+      <c r="AI49" s="51"/>
+      <c r="AJ49" s="39"/>
+      <c r="AK49" s="39"/>
+      <c r="AL49" s="51"/>
+      <c r="AM49" s="51"/>
+      <c r="AN49" s="38"/>
+      <c r="AO49" s="39"/>
+      <c r="AP49" s="39"/>
+      <c r="AQ49" s="39"/>
+      <c r="AR49" s="39"/>
+      <c r="AS49" s="51"/>
+      <c r="AT49" s="52"/>
+      <c r="AU49" s="38"/>
+      <c r="AV49" s="28"/>
+      <c r="AW49" s="39"/>
+      <c r="AX49" s="40"/>
+      <c r="AY49" s="40"/>
+      <c r="AZ49" s="40"/>
+      <c r="BA49" s="41"/>
+    </row>
+    <row r="50" spans="1:53">
+      <c r="A50" s="116"/>
+      <c r="B50" s="107" t="s">
         <v>86</v>
       </c>
       <c r="C50" s="60" t="s">
         <v>87</v>
       </c>
       <c r="D50" s="92">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E50" s="74" t="s">
         <v>88</v>
@@ -4556,15 +4931,57 @@
       <c r="H50" s="31"/>
       <c r="I50" s="31"/>
       <c r="J50" s="31"/>
-    </row>
-    <row r="51" spans="1:49">
-      <c r="A51" s="111"/>
-      <c r="B51" s="114"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="39"/>
+      <c r="T50" s="39"/>
+      <c r="U50" s="39"/>
+      <c r="V50" s="39"/>
+      <c r="W50" s="39"/>
+      <c r="X50" s="51"/>
+      <c r="Y50" s="51"/>
+      <c r="Z50" s="38"/>
+      <c r="AA50" s="39"/>
+      <c r="AB50" s="39"/>
+      <c r="AC50" s="39"/>
+      <c r="AD50" s="39"/>
+      <c r="AE50" s="51"/>
+      <c r="AF50" s="52"/>
+      <c r="AG50" s="51"/>
+      <c r="AH50" s="51"/>
+      <c r="AI50" s="51"/>
+      <c r="AJ50" s="39"/>
+      <c r="AK50" s="39"/>
+      <c r="AL50" s="51"/>
+      <c r="AM50" s="51"/>
+      <c r="AN50" s="38"/>
+      <c r="AO50" s="39"/>
+      <c r="AP50" s="39"/>
+      <c r="AQ50" s="39"/>
+      <c r="AR50" s="39"/>
+      <c r="AS50" s="51"/>
+      <c r="AT50" s="52"/>
+      <c r="AU50" s="38"/>
+      <c r="AV50" s="28"/>
+      <c r="AW50" s="39"/>
+      <c r="AX50" s="40"/>
+      <c r="AY50" s="40"/>
+      <c r="AZ50" s="40"/>
+      <c r="BA50" s="41"/>
+    </row>
+    <row r="51" spans="1:53">
+      <c r="A51" s="116"/>
+      <c r="B51" s="108"/>
       <c r="C51" s="59" t="s">
         <v>89</v>
       </c>
       <c r="D51" s="95">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E51" s="76" t="s">
         <v>19</v>
@@ -4576,17 +4993,59 @@
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
-    </row>
-    <row r="52" spans="1:49">
-      <c r="A52" s="111"/>
-      <c r="B52" s="116" t="s">
+      <c r="L51" s="38"/>
+      <c r="M51" s="39"/>
+      <c r="N51" s="39"/>
+      <c r="O51" s="39"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="46"/>
+      <c r="S51" s="39"/>
+      <c r="T51" s="39"/>
+      <c r="U51" s="39"/>
+      <c r="V51" s="39"/>
+      <c r="W51" s="39"/>
+      <c r="X51" s="51"/>
+      <c r="Y51" s="51"/>
+      <c r="Z51" s="38"/>
+      <c r="AA51" s="39"/>
+      <c r="AB51" s="39"/>
+      <c r="AC51" s="39"/>
+      <c r="AD51" s="39"/>
+      <c r="AE51" s="51"/>
+      <c r="AF51" s="52"/>
+      <c r="AG51" s="51"/>
+      <c r="AH51" s="51"/>
+      <c r="AI51" s="51"/>
+      <c r="AJ51" s="39"/>
+      <c r="AK51" s="39"/>
+      <c r="AL51" s="51"/>
+      <c r="AM51" s="51"/>
+      <c r="AN51" s="38"/>
+      <c r="AO51" s="39"/>
+      <c r="AP51" s="39"/>
+      <c r="AQ51" s="39"/>
+      <c r="AR51" s="39"/>
+      <c r="AS51" s="51"/>
+      <c r="AT51" s="52"/>
+      <c r="AU51" s="38"/>
+      <c r="AV51" s="28"/>
+      <c r="AW51" s="39"/>
+      <c r="AX51" s="40"/>
+      <c r="AY51" s="40"/>
+      <c r="AZ51" s="40"/>
+      <c r="BA51" s="41"/>
+    </row>
+    <row r="52" spans="1:53">
+      <c r="A52" s="116"/>
+      <c r="B52" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="116" t="s">
+      <c r="C52" s="113" t="s">
         <v>91</v>
       </c>
-      <c r="D52" s="99">
-        <v>25</v>
+      <c r="D52" s="119">
+        <v>29</v>
       </c>
       <c r="E52" s="74" t="s">
         <v>92</v>
@@ -4598,12 +5057,54 @@
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:49">
-      <c r="A53" s="111"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="100"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="39"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="45"/>
+      <c r="R52" s="46"/>
+      <c r="S52" s="39"/>
+      <c r="T52" s="39"/>
+      <c r="U52" s="39"/>
+      <c r="V52" s="39"/>
+      <c r="W52" s="39"/>
+      <c r="X52" s="51"/>
+      <c r="Y52" s="51"/>
+      <c r="Z52" s="38"/>
+      <c r="AA52" s="39"/>
+      <c r="AB52" s="39"/>
+      <c r="AC52" s="39"/>
+      <c r="AD52" s="39"/>
+      <c r="AE52" s="51"/>
+      <c r="AF52" s="52"/>
+      <c r="AG52" s="51"/>
+      <c r="AH52" s="51"/>
+      <c r="AI52" s="51"/>
+      <c r="AJ52" s="39"/>
+      <c r="AK52" s="39"/>
+      <c r="AL52" s="51"/>
+      <c r="AM52" s="51"/>
+      <c r="AN52" s="38"/>
+      <c r="AO52" s="39"/>
+      <c r="AP52" s="39"/>
+      <c r="AQ52" s="39"/>
+      <c r="AR52" s="39"/>
+      <c r="AS52" s="51"/>
+      <c r="AT52" s="52"/>
+      <c r="AU52" s="38"/>
+      <c r="AV52" s="28"/>
+      <c r="AW52" s="39"/>
+      <c r="AX52" s="40"/>
+      <c r="AY52" s="40"/>
+      <c r="AZ52" s="40"/>
+      <c r="BA52" s="41"/>
+    </row>
+    <row r="53" spans="1:53">
+      <c r="A53" s="116"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="120"/>
       <c r="E53" s="31" t="s">
         <v>64</v>
       </c>
@@ -4614,17 +5115,59 @@
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
       <c r="J53" s="70"/>
-    </row>
-    <row r="54" spans="1:49">
-      <c r="A54" s="111"/>
-      <c r="B54" s="109" t="s">
+      <c r="L53" s="38"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="39"/>
+      <c r="O53" s="39"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="45"/>
+      <c r="R53" s="46"/>
+      <c r="S53" s="39"/>
+      <c r="T53" s="39"/>
+      <c r="U53" s="39"/>
+      <c r="V53" s="39"/>
+      <c r="W53" s="39"/>
+      <c r="X53" s="51"/>
+      <c r="Y53" s="51"/>
+      <c r="Z53" s="38"/>
+      <c r="AA53" s="39"/>
+      <c r="AB53" s="39"/>
+      <c r="AC53" s="39"/>
+      <c r="AD53" s="39"/>
+      <c r="AE53" s="51"/>
+      <c r="AF53" s="52"/>
+      <c r="AG53" s="51"/>
+      <c r="AH53" s="51"/>
+      <c r="AI53" s="51"/>
+      <c r="AJ53" s="39"/>
+      <c r="AK53" s="39"/>
+      <c r="AL53" s="51"/>
+      <c r="AM53" s="51"/>
+      <c r="AN53" s="38"/>
+      <c r="AO53" s="39"/>
+      <c r="AP53" s="39"/>
+      <c r="AQ53" s="39"/>
+      <c r="AR53" s="39"/>
+      <c r="AS53" s="51"/>
+      <c r="AT53" s="52"/>
+      <c r="AU53" s="38"/>
+      <c r="AV53" s="28"/>
+      <c r="AW53" s="39"/>
+      <c r="AX53" s="40"/>
+      <c r="AY53" s="40"/>
+      <c r="AZ53" s="40"/>
+      <c r="BA53" s="41"/>
+    </row>
+    <row r="54" spans="1:53">
+      <c r="A54" s="116"/>
+      <c r="B54" s="114" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="101">
-        <v>26</v>
+      <c r="D54" s="96">
+        <v>30</v>
       </c>
       <c r="E54" s="31" t="s">
         <v>95</v>
@@ -4637,16 +5180,58 @@
       <c r="I54" s="31"/>
       <c r="J54" s="31"/>
       <c r="K54" s="29"/>
-      <c r="AV54" s="12"/>
-      <c r="AW54" s="12"/>
-    </row>
-    <row r="55" spans="1:49">
-      <c r="A55" s="112"/>
-      <c r="B55" s="109"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="39"/>
+      <c r="O54" s="39"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="45"/>
+      <c r="R54" s="46"/>
+      <c r="S54" s="39"/>
+      <c r="T54" s="39"/>
+      <c r="U54" s="39"/>
+      <c r="V54" s="39"/>
+      <c r="W54" s="39"/>
+      <c r="X54" s="51"/>
+      <c r="Y54" s="51"/>
+      <c r="Z54" s="38"/>
+      <c r="AA54" s="39"/>
+      <c r="AB54" s="39"/>
+      <c r="AC54" s="39"/>
+      <c r="AD54" s="39"/>
+      <c r="AE54" s="51"/>
+      <c r="AF54" s="52"/>
+      <c r="AG54" s="51"/>
+      <c r="AH54" s="51"/>
+      <c r="AI54" s="51"/>
+      <c r="AJ54" s="39"/>
+      <c r="AK54" s="39"/>
+      <c r="AL54" s="51"/>
+      <c r="AM54" s="51"/>
+      <c r="AN54" s="38"/>
+      <c r="AO54" s="39"/>
+      <c r="AP54" s="39"/>
+      <c r="AQ54" s="39"/>
+      <c r="AR54" s="39"/>
+      <c r="AS54" s="51"/>
+      <c r="AT54" s="52"/>
+      <c r="AU54" s="38"/>
+      <c r="AV54" s="28"/>
+      <c r="AW54" s="39"/>
+      <c r="AX54" s="40"/>
+      <c r="AY54" s="40"/>
+      <c r="AZ54" s="40"/>
+      <c r="BA54" s="41"/>
+    </row>
+    <row r="55" spans="1:53">
+      <c r="A55" s="117"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="102"/>
+      <c r="D55" s="96">
+        <v>31</v>
+      </c>
       <c r="E55" s="9" t="s">
         <v>98</v>
       </c>
@@ -4657,13 +5242,98 @@
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
-    </row>
-    <row r="56" spans="1:49">
+      <c r="L55" s="38"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="45"/>
+      <c r="R55" s="46"/>
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="39"/>
+      <c r="V55" s="39"/>
+      <c r="W55" s="39"/>
+      <c r="X55" s="51"/>
+      <c r="Y55" s="51"/>
+      <c r="Z55" s="38"/>
+      <c r="AA55" s="39"/>
+      <c r="AB55" s="39"/>
+      <c r="AC55" s="39"/>
+      <c r="AD55" s="39"/>
+      <c r="AE55" s="51"/>
+      <c r="AF55" s="52"/>
+      <c r="AG55" s="51"/>
+      <c r="AH55" s="51"/>
+      <c r="AI55" s="51"/>
+      <c r="AJ55" s="39"/>
+      <c r="AK55" s="39"/>
+      <c r="AL55" s="51"/>
+      <c r="AM55" s="51"/>
+      <c r="AN55" s="38"/>
+      <c r="AO55" s="39"/>
+      <c r="AP55" s="39"/>
+      <c r="AQ55" s="39"/>
+      <c r="AR55" s="39"/>
+      <c r="AS55" s="51"/>
+      <c r="AT55" s="52"/>
+      <c r="AU55" s="38"/>
+      <c r="AV55" s="28"/>
+      <c r="AW55" s="39"/>
+      <c r="AX55" s="40"/>
+      <c r="AY55" s="40"/>
+      <c r="AZ55" s="40"/>
+      <c r="BA55" s="41"/>
+    </row>
+    <row r="56" spans="1:53">
       <c r="K56" s="29"/>
       <c r="AW56" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="59">
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A45:A55"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B23:B27"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="C11:C12"/>
@@ -4680,50 +5350,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B3:B16"/>
     <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WBS File Modified by JongSeong
</commit_message>
<xml_diff>
--- a/결과물/WBS.xlsx
+++ b/결과물/WBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woo/Desktop/Boostcamp_3th/gitflowex/결과물/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\카퀴카퀴\Desktop\수업\부스트캠프\TeamH 아카이브\boostcamp3_archive\결과물\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390D913D-EFFB-8940-AF3E-9D755079AF63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5432D1-1B32-411D-A0EB-68651F892EC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="17544" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -814,7 +814,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1106,6 +1106,114 @@
     <xf numFmtId="178" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1115,15 +1223,6 @@
     <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1133,103 +1232,28 @@
     <xf numFmtId="178" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1558,7 +1582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,59 +1594,59 @@
   <dimension ref="A1:DA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z29" sqref="Z29"/>
+      <selection pane="bottomRight" activeCell="Q22" sqref="Q22:R26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="9" style="12"/>
     <col min="2" max="3" width="16" style="12" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="91" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" style="91" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="12" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.296875" style="12" customWidth="1"/>
     <col min="7" max="7" width="8" style="12" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.796875" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="0" style="12" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="12"/>
-    <col min="11" max="11" width="3.6640625" style="12" customWidth="1"/>
-    <col min="12" max="49" width="2.33203125" style="29" customWidth="1"/>
-    <col min="50" max="53" width="2.33203125" style="12" customWidth="1"/>
-    <col min="54" max="115" width="3.1640625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="3.69921875" style="12" customWidth="1"/>
+    <col min="12" max="49" width="2.296875" style="29" customWidth="1"/>
+    <col min="50" max="53" width="2.296875" style="12" customWidth="1"/>
+    <col min="54" max="115" width="3.19921875" style="12" customWidth="1"/>
     <col min="116" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:105">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="106" t="s">
+      <c r="J1" s="109" t="s">
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1735,16 +1759,16 @@
       <c r="DA1" s="14"/>
     </row>
     <row r="2" spans="1:105">
-      <c r="A2" s="122"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
+      <c r="A2" s="114"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
       <c r="L2" s="16">
         <v>43486</v>
       </c>
@@ -1925,16 +1949,16 @@
       <c r="DA2" s="19"/>
     </row>
     <row r="3" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="116" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="102">
+      <c r="D3" s="130">
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1961,8 +1985,8 @@
       <c r="R3" s="44"/>
       <c r="S3" s="20"/>
       <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
       <c r="W3" s="21"/>
       <c r="X3" s="49"/>
       <c r="Y3" s="50"/>
@@ -2048,10 +2072,10 @@
       <c r="DA3" s="24"/>
     </row>
     <row r="4" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A4" s="123"/>
-      <c r="B4" s="125"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="100"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="131"/>
       <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2072,8 +2096,8 @@
       <c r="R4" s="44"/>
       <c r="S4" s="20"/>
       <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
       <c r="W4" s="21"/>
       <c r="X4" s="49"/>
       <c r="Y4" s="50"/>
@@ -2159,10 +2183,10 @@
       <c r="DA4" s="24"/>
     </row>
     <row r="5" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A5" s="123"/>
-      <c r="B5" s="125"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="100"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="131"/>
       <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
@@ -2183,8 +2207,8 @@
       <c r="R5" s="44"/>
       <c r="S5" s="20"/>
       <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
+      <c r="U5" s="139"/>
+      <c r="V5" s="139"/>
       <c r="W5" s="21"/>
       <c r="X5" s="49"/>
       <c r="Y5" s="50"/>
@@ -2270,10 +2294,10 @@
       <c r="DA5" s="24"/>
     </row>
     <row r="6" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A6" s="123"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="101"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
@@ -2297,8 +2321,8 @@
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
       <c r="W6" s="21"/>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="50"/>
+      <c r="X6" s="139"/>
+      <c r="Y6" s="140"/>
       <c r="Z6" s="20"/>
       <c r="AA6" s="21"/>
       <c r="AB6" s="21"/>
@@ -2381,12 +2405,12 @@
       <c r="DA6" s="24"/>
     </row>
     <row r="7" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A7" s="123"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="116" t="s">
+      <c r="A7" s="115"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="102">
+      <c r="D7" s="130">
         <v>4</v>
       </c>
       <c r="E7" s="77" t="s">
@@ -2411,7 +2435,7 @@
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
       <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
+      <c r="W7" s="139"/>
       <c r="X7" s="49"/>
       <c r="Y7" s="50"/>
       <c r="Z7" s="20"/>
@@ -2496,10 +2520,10 @@
       <c r="DA7" s="24"/>
     </row>
     <row r="8" spans="1:105" ht="16.5" customHeight="1" outlineLevel="1">
-      <c r="A8" s="123"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="100"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="72" t="s">
         <v>27</v>
       </c>
@@ -2522,7 +2546,7 @@
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
       <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
+      <c r="W8" s="139"/>
       <c r="X8" s="49"/>
       <c r="Y8" s="50"/>
       <c r="Z8" s="20"/>
@@ -2606,11 +2630,11 @@
       <c r="CZ8" s="24"/>
       <c r="DA8" s="24"/>
     </row>
-    <row r="9" spans="1:105" ht="18.5" customHeight="1">
-      <c r="A9" s="123"/>
-      <c r="B9" s="125"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="101"/>
+    <row r="9" spans="1:105" ht="18.45" customHeight="1">
+      <c r="A9" s="115"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="76" t="s">
         <v>28</v>
       </c>
@@ -2626,20 +2650,20 @@
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="141"/>
+      <c r="T9" s="142"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
       <c r="AE9" s="49"/>
       <c r="AF9" s="50"/>
       <c r="AG9" s="56"/>
@@ -2665,8 +2689,8 @@
       <c r="BA9" s="22"/>
     </row>
     <row r="10" spans="1:105">
-      <c r="A10" s="123"/>
-      <c r="B10" s="125"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="60" t="s">
         <v>18</v>
       </c>
@@ -2688,20 +2712,20 @@
       <c r="N10" s="21"/>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="49"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="53"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="143"/>
+      <c r="AC10" s="143"/>
+      <c r="AD10" s="33"/>
       <c r="AE10" s="49"/>
       <c r="AF10" s="50"/>
       <c r="AG10" s="56"/>
@@ -2727,12 +2751,12 @@
       <c r="BA10" s="22"/>
     </row>
     <row r="11" spans="1:105">
-      <c r="A11" s="123"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="116" t="s">
+      <c r="A11" s="115"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="102">
+      <c r="D11" s="130">
         <v>8</v>
       </c>
       <c r="E11" s="77" t="s">
@@ -2760,8 +2784,8 @@
       <c r="W11" s="21"/>
       <c r="X11" s="49"/>
       <c r="Y11" s="50"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="21"/>
+      <c r="Z11" s="144"/>
+      <c r="AA11" s="139"/>
       <c r="AB11" s="21"/>
       <c r="AC11" s="21"/>
       <c r="AD11" s="21"/>
@@ -2790,10 +2814,10 @@
       <c r="BA11" s="22"/>
     </row>
     <row r="12" spans="1:105">
-      <c r="A12" s="123"/>
-      <c r="B12" s="125"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="101"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="132"/>
       <c r="E12" s="65" t="s">
         <v>32</v>
       </c>
@@ -2818,8 +2842,8 @@
       <c r="W12" s="21"/>
       <c r="X12" s="49"/>
       <c r="Y12" s="50"/>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="21"/>
+      <c r="Z12" s="144"/>
+      <c r="AA12" s="139"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
       <c r="AD12" s="21"/>
@@ -2848,12 +2872,12 @@
       <c r="BA12" s="22"/>
     </row>
     <row r="13" spans="1:105">
-      <c r="A13" s="123"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="116" t="s">
+      <c r="A13" s="115"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="102">
+      <c r="D13" s="130">
         <v>9</v>
       </c>
       <c r="E13" s="77" t="s">
@@ -2910,10 +2934,10 @@
       <c r="BA13" s="27"/>
     </row>
     <row r="14" spans="1:105">
-      <c r="A14" s="123"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="101"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="132"/>
       <c r="E14" s="77" t="s">
         <v>35</v>
       </c>
@@ -2967,13 +2991,13 @@
       <c r="AZ14" s="33"/>
       <c r="BA14" s="34"/>
     </row>
-    <row r="15" spans="1:105" ht="15.5" customHeight="1">
-      <c r="A15" s="123"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="116" t="s">
+    <row r="15" spans="1:105" ht="15.45" customHeight="1">
+      <c r="A15" s="115"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="102">
+      <c r="D15" s="130">
         <v>10</v>
       </c>
       <c r="E15" s="75" t="s">
@@ -3031,10 +3055,10 @@
       <c r="BA15" s="22"/>
     </row>
     <row r="16" spans="1:105">
-      <c r="A16" s="123"/>
-      <c r="B16" s="126"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="101"/>
+      <c r="A16" s="115"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="132"/>
       <c r="E16" s="76" t="s">
         <v>38</v>
       </c>
@@ -3090,14 +3114,14 @@
       <c r="BA16" s="22"/>
     </row>
     <row r="17" spans="1:53">
-      <c r="A17" s="123"/>
-      <c r="B17" s="112" t="s">
+      <c r="A17" s="115"/>
+      <c r="B17" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="102">
+      <c r="D17" s="130">
         <v>11</v>
       </c>
       <c r="E17" s="77" t="s">
@@ -3157,10 +3181,10 @@
       <c r="BA17" s="22"/>
     </row>
     <row r="18" spans="1:53">
-      <c r="A18" s="123"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="100"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="131"/>
       <c r="E18" s="77" t="s">
         <v>42</v>
       </c>
@@ -3215,10 +3239,10 @@
       <c r="BA18" s="22"/>
     </row>
     <row r="19" spans="1:53">
-      <c r="A19" s="123"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="101"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="132"/>
       <c r="E19" s="66" t="s">
         <v>43</v>
       </c>
@@ -3273,12 +3297,12 @@
       <c r="BA19" s="22"/>
     </row>
     <row r="20" spans="1:53">
-      <c r="A20" s="123"/>
-      <c r="B20" s="113"/>
-      <c r="C20" s="112" t="s">
+      <c r="A20" s="115"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="97">
+      <c r="D20" s="133">
         <v>12</v>
       </c>
       <c r="E20" s="77" t="s">
@@ -3328,10 +3352,10 @@
       <c r="BA20" s="7"/>
     </row>
     <row r="21" spans="1:53">
-      <c r="A21" s="123"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="98"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="134"/>
       <c r="E21" s="77" t="s">
         <v>42</v>
       </c>
@@ -3379,10 +3403,10 @@
       <c r="BA21" s="7"/>
     </row>
     <row r="22" spans="1:53">
-      <c r="A22" s="123"/>
-      <c r="B22" s="114"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="99"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="135"/>
       <c r="E22" s="76" t="s">
         <v>43</v>
       </c>
@@ -3398,8 +3422,8 @@
       <c r="N22" s="37"/>
       <c r="O22" s="37"/>
       <c r="P22" s="37"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="44"/>
+      <c r="Q22" s="145"/>
+      <c r="R22" s="146"/>
       <c r="X22" s="55"/>
       <c r="Y22" s="55"/>
       <c r="Z22" s="36"/>
@@ -3430,14 +3454,14 @@
       <c r="BA22" s="7"/>
     </row>
     <row r="23" spans="1:53">
-      <c r="A23" s="123"/>
-      <c r="B23" s="112" t="s">
+      <c r="A23" s="115"/>
+      <c r="B23" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="102">
+      <c r="D23" s="130">
         <v>13</v>
       </c>
       <c r="E23" s="77" t="s">
@@ -3457,8 +3481,8 @@
       <c r="N23" s="37"/>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="44"/>
+      <c r="Q23" s="145"/>
+      <c r="R23" s="146"/>
       <c r="X23" s="55"/>
       <c r="Y23" s="55"/>
       <c r="Z23" s="36"/>
@@ -3489,10 +3513,10 @@
       <c r="BA23" s="7"/>
     </row>
     <row r="24" spans="1:53">
-      <c r="A24" s="123"/>
-      <c r="B24" s="113"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="100"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="131"/>
       <c r="E24" s="61" t="s">
         <v>47</v>
       </c>
@@ -3508,8 +3532,8 @@
       <c r="N24" s="37"/>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="44"/>
+      <c r="Q24" s="145"/>
+      <c r="R24" s="146"/>
       <c r="X24" s="55"/>
       <c r="Y24" s="55"/>
       <c r="Z24" s="36"/>
@@ -3540,10 +3564,10 @@
       <c r="BA24" s="7"/>
     </row>
     <row r="25" spans="1:53">
-      <c r="A25" s="123"/>
-      <c r="B25" s="113"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="101"/>
+      <c r="A25" s="115"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="132"/>
       <c r="E25" s="78" t="s">
         <v>48</v>
       </c>
@@ -3559,8 +3583,8 @@
       <c r="N25" s="37"/>
       <c r="O25" s="37"/>
       <c r="P25" s="37"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="44"/>
+      <c r="Q25" s="145"/>
+      <c r="R25" s="146"/>
       <c r="X25" s="55"/>
       <c r="Y25" s="55"/>
       <c r="Z25" s="36"/>
@@ -3591,12 +3615,12 @@
       <c r="BA25" s="7"/>
     </row>
     <row r="26" spans="1:53">
-      <c r="A26" s="123"/>
-      <c r="B26" s="113"/>
-      <c r="C26" s="116" t="s">
+      <c r="A26" s="115"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="102">
+      <c r="D26" s="130">
         <v>14</v>
       </c>
       <c r="E26" s="73" t="s">
@@ -3614,8 +3638,8 @@
       <c r="N26" s="37"/>
       <c r="O26" s="37"/>
       <c r="P26" s="37"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
+      <c r="Q26" s="145"/>
+      <c r="R26" s="146"/>
       <c r="X26" s="55"/>
       <c r="Y26" s="55"/>
       <c r="Z26" s="36"/>
@@ -3646,10 +3670,10 @@
       <c r="BA26" s="7"/>
     </row>
     <row r="27" spans="1:53">
-      <c r="A27" s="123"/>
-      <c r="B27" s="114"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="101"/>
+      <c r="A27" s="115"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="132"/>
       <c r="E27" s="76" t="s">
         <v>51</v>
       </c>
@@ -3697,8 +3721,8 @@
       <c r="BA27" s="7"/>
     </row>
     <row r="28" spans="1:53">
-      <c r="A28" s="123"/>
-      <c r="B28" s="112" t="s">
+      <c r="A28" s="115"/>
+      <c r="B28" s="119" t="s">
         <v>56</v>
       </c>
       <c r="C28" s="60" t="s">
@@ -3728,15 +3752,15 @@
       <c r="R28" s="44"/>
       <c r="X28" s="55"/>
       <c r="Y28" s="55"/>
-      <c r="Z28" s="136" t="s">
+      <c r="Z28" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="AA28" s="137"/>
-      <c r="AB28" s="137"/>
-      <c r="AC28" s="137"/>
-      <c r="AD28" s="137"/>
-      <c r="AE28" s="137"/>
-      <c r="AF28" s="138"/>
+      <c r="AA28" s="107"/>
+      <c r="AB28" s="107"/>
+      <c r="AC28" s="107"/>
+      <c r="AD28" s="107"/>
+      <c r="AE28" s="107"/>
+      <c r="AF28" s="108"/>
       <c r="AG28" s="55"/>
       <c r="AH28" s="55"/>
       <c r="AI28" s="55"/>
@@ -3758,12 +3782,12 @@
       <c r="BA28" s="7"/>
     </row>
     <row r="29" spans="1:53">
-      <c r="A29" s="123"/>
-      <c r="B29" s="113"/>
-      <c r="C29" s="116" t="s">
+      <c r="A29" s="115"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="102">
+      <c r="D29" s="130">
         <v>16</v>
       </c>
       <c r="E29" s="75" t="s">
@@ -3785,13 +3809,13 @@
       <c r="R29" s="44"/>
       <c r="X29" s="55"/>
       <c r="Y29" s="55"/>
-      <c r="Z29" s="133"/>
-      <c r="AA29" s="134"/>
-      <c r="AB29" s="134"/>
-      <c r="AC29" s="134"/>
-      <c r="AD29" s="134"/>
-      <c r="AE29" s="134"/>
-      <c r="AF29" s="135"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="101"/>
+      <c r="AD29" s="101"/>
+      <c r="AE29" s="101"/>
+      <c r="AF29" s="102"/>
       <c r="AG29" s="55"/>
       <c r="AH29" s="55"/>
       <c r="AI29" s="55"/>
@@ -3813,10 +3837,10 @@
       <c r="BA29" s="7"/>
     </row>
     <row r="30" spans="1:53">
-      <c r="A30" s="123"/>
-      <c r="B30" s="113"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="100"/>
+      <c r="A30" s="115"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="131"/>
       <c r="E30" s="77" t="s">
         <v>41</v>
       </c>
@@ -3836,13 +3860,13 @@
       <c r="R30" s="44"/>
       <c r="X30" s="55"/>
       <c r="Y30" s="55"/>
-      <c r="Z30" s="133"/>
-      <c r="AA30" s="134"/>
-      <c r="AB30" s="134"/>
-      <c r="AC30" s="134"/>
-      <c r="AD30" s="134"/>
-      <c r="AE30" s="134"/>
-      <c r="AF30" s="135"/>
+      <c r="Z30" s="100"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="101"/>
+      <c r="AC30" s="101"/>
+      <c r="AD30" s="101"/>
+      <c r="AE30" s="101"/>
+      <c r="AF30" s="102"/>
       <c r="AG30" s="55"/>
       <c r="AH30" s="55"/>
       <c r="AI30" s="55"/>
@@ -3864,10 +3888,10 @@
       <c r="BA30" s="7"/>
     </row>
     <row r="31" spans="1:53">
-      <c r="A31" s="123"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="101"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="121"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="132"/>
       <c r="E31" s="76" t="s">
         <v>55</v>
       </c>
@@ -3887,13 +3911,13 @@
       <c r="R31" s="44"/>
       <c r="X31" s="55"/>
       <c r="Y31" s="55"/>
-      <c r="Z31" s="133"/>
-      <c r="AA31" s="134"/>
-      <c r="AB31" s="134"/>
-      <c r="AC31" s="134"/>
-      <c r="AD31" s="134"/>
-      <c r="AE31" s="134"/>
-      <c r="AF31" s="135"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="101"/>
+      <c r="AB31" s="101"/>
+      <c r="AC31" s="101"/>
+      <c r="AD31" s="101"/>
+      <c r="AE31" s="101"/>
+      <c r="AF31" s="102"/>
       <c r="AG31" s="55"/>
       <c r="AH31" s="55"/>
       <c r="AI31" s="55"/>
@@ -3915,16 +3939,16 @@
       <c r="BA31" s="7"/>
     </row>
     <row r="32" spans="1:53">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="112" t="s">
+      <c r="B32" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="116" t="s">
+      <c r="C32" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="102">
+      <c r="D32" s="130">
         <v>17</v>
       </c>
       <c r="E32" s="58" t="s">
@@ -3976,10 +4000,10 @@
       <c r="BA32" s="7"/>
     </row>
     <row r="33" spans="1:53">
-      <c r="A33" s="113"/>
-      <c r="B33" s="113"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="101"/>
+      <c r="A33" s="120"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="113"/>
+      <c r="D33" s="132"/>
       <c r="E33" s="76" t="s">
         <v>23</v>
       </c>
@@ -4026,9 +4050,9 @@
       <c r="AZ33" s="6"/>
       <c r="BA33" s="7"/>
     </row>
-    <row r="34" spans="1:53" ht="30">
-      <c r="A34" s="113"/>
-      <c r="B34" s="113"/>
+    <row r="34" spans="1:53" ht="26.4">
+      <c r="A34" s="120"/>
+      <c r="B34" s="120"/>
       <c r="C34" s="60" t="s">
         <v>61</v>
       </c>
@@ -4082,12 +4106,12 @@
       <c r="BA34" s="7"/>
     </row>
     <row r="35" spans="1:53">
-      <c r="A35" s="113"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="116" t="s">
+      <c r="A35" s="120"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="102">
+      <c r="D35" s="130">
         <v>19</v>
       </c>
       <c r="E35" s="68" t="s">
@@ -4137,10 +4161,10 @@
       <c r="BA35" s="7"/>
     </row>
     <row r="36" spans="1:53">
-      <c r="A36" s="113"/>
-      <c r="B36" s="113"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="101"/>
+      <c r="A36" s="120"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="132"/>
       <c r="E36" s="62" t="s">
         <v>64</v>
       </c>
@@ -4188,8 +4212,8 @@
       <c r="BA36" s="7"/>
     </row>
     <row r="37" spans="1:53">
-      <c r="A37" s="113"/>
-      <c r="B37" s="114"/>
+      <c r="A37" s="120"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="60" t="s">
         <v>65</v>
       </c>
@@ -4243,8 +4267,8 @@
       <c r="BA37" s="7"/>
     </row>
     <row r="38" spans="1:53">
-      <c r="A38" s="113"/>
-      <c r="B38" s="112" t="s">
+      <c r="A38" s="120"/>
+      <c r="B38" s="119" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="60" t="s">
@@ -4300,12 +4324,12 @@
       <c r="BA38" s="7"/>
     </row>
     <row r="39" spans="1:53">
-      <c r="A39" s="113"/>
-      <c r="B39" s="113"/>
-      <c r="C39" s="119" t="s">
+      <c r="A39" s="120"/>
+      <c r="B39" s="120"/>
+      <c r="C39" s="122" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="103">
+      <c r="D39" s="136">
         <v>22</v>
       </c>
       <c r="E39" s="57" t="s">
@@ -4355,10 +4379,10 @@
       <c r="BA39" s="7"/>
     </row>
     <row r="40" spans="1:53">
-      <c r="A40" s="113"/>
-      <c r="B40" s="113"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="104"/>
+      <c r="A40" s="120"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="123"/>
+      <c r="D40" s="137"/>
       <c r="E40" s="77" t="s">
         <v>70</v>
       </c>
@@ -4413,10 +4437,10 @@
       <c r="BA40" s="41"/>
     </row>
     <row r="41" spans="1:53">
-      <c r="A41" s="114"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="121"/>
-      <c r="D41" s="105"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="124"/>
+      <c r="D41" s="138"/>
       <c r="E41" s="76" t="s">
         <v>71</v>
       </c>
@@ -4471,10 +4495,10 @@
       <c r="BA41" s="41"/>
     </row>
     <row r="42" spans="1:53">
-      <c r="A42" s="112" t="s">
+      <c r="A42" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="113" t="s">
+      <c r="B42" s="120" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="60" t="s">
@@ -4502,15 +4526,15 @@
       <c r="P42" s="39"/>
       <c r="Q42" s="45"/>
       <c r="R42" s="46"/>
-      <c r="S42" s="128" t="s">
+      <c r="S42" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="T42" s="129"/>
-      <c r="U42" s="129"/>
-      <c r="V42" s="129"/>
-      <c r="W42" s="129"/>
-      <c r="X42" s="129"/>
-      <c r="Y42" s="130"/>
+      <c r="T42" s="104"/>
+      <c r="U42" s="104"/>
+      <c r="V42" s="104"/>
+      <c r="W42" s="104"/>
+      <c r="X42" s="104"/>
+      <c r="Y42" s="105"/>
       <c r="Z42" s="38"/>
       <c r="AA42" s="39"/>
       <c r="AB42" s="39"/>
@@ -4541,12 +4565,12 @@
       <c r="BA42" s="41"/>
     </row>
     <row r="43" spans="1:53">
-      <c r="A43" s="113"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113" t="s">
+      <c r="A43" s="120"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="97">
+      <c r="D43" s="133">
         <v>24</v>
       </c>
       <c r="E43" s="75" t="s">
@@ -4566,13 +4590,13 @@
       <c r="P43" s="39"/>
       <c r="Q43" s="45"/>
       <c r="R43" s="46"/>
-      <c r="S43" s="127"/>
-      <c r="T43" s="127"/>
-      <c r="U43" s="127"/>
-      <c r="V43" s="127"/>
-      <c r="W43" s="127"/>
-      <c r="X43" s="127"/>
-      <c r="Y43" s="127"/>
+      <c r="S43" s="97"/>
+      <c r="T43" s="97"/>
+      <c r="U43" s="97"/>
+      <c r="V43" s="97"/>
+      <c r="W43" s="97"/>
+      <c r="X43" s="97"/>
+      <c r="Y43" s="97"/>
       <c r="Z43" s="38"/>
       <c r="AA43" s="39"/>
       <c r="AB43" s="39"/>
@@ -4603,10 +4627,10 @@
       <c r="BA43" s="41"/>
     </row>
     <row r="44" spans="1:53">
-      <c r="A44" s="114"/>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="99"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="135"/>
       <c r="E44" s="76" t="s">
         <v>77</v>
       </c>
@@ -4624,13 +4648,13 @@
       <c r="P44" s="39"/>
       <c r="Q44" s="45"/>
       <c r="R44" s="46"/>
-      <c r="S44" s="127"/>
-      <c r="T44" s="127"/>
-      <c r="U44" s="127"/>
-      <c r="V44" s="127"/>
-      <c r="W44" s="127"/>
-      <c r="X44" s="127"/>
-      <c r="Y44" s="127"/>
+      <c r="S44" s="97"/>
+      <c r="T44" s="97"/>
+      <c r="U44" s="97"/>
+      <c r="V44" s="97"/>
+      <c r="W44" s="97"/>
+      <c r="X44" s="97"/>
+      <c r="Y44" s="97"/>
       <c r="Z44" s="38"/>
       <c r="AA44" s="39"/>
       <c r="AB44" s="39"/>
@@ -4661,16 +4685,16 @@
       <c r="BA44" s="41"/>
     </row>
     <row r="45" spans="1:53">
-      <c r="A45" s="109" t="s">
+      <c r="A45" s="127" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="113" t="s">
+      <c r="B45" s="120" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="112" t="s">
+      <c r="C45" s="119" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="97">
+      <c r="D45" s="133">
         <v>25</v>
       </c>
       <c r="E45" s="75" t="s">
@@ -4690,13 +4714,13 @@
       <c r="P45" s="39"/>
       <c r="Q45" s="45"/>
       <c r="R45" s="46"/>
-      <c r="S45" s="127"/>
-      <c r="T45" s="127"/>
-      <c r="U45" s="127"/>
-      <c r="V45" s="127"/>
-      <c r="W45" s="127"/>
-      <c r="X45" s="127"/>
-      <c r="Y45" s="127"/>
+      <c r="S45" s="97"/>
+      <c r="T45" s="97"/>
+      <c r="U45" s="97"/>
+      <c r="V45" s="97"/>
+      <c r="W45" s="97"/>
+      <c r="X45" s="97"/>
+      <c r="Y45" s="97"/>
       <c r="Z45" s="38"/>
       <c r="AA45" s="39"/>
       <c r="AB45" s="39"/>
@@ -4727,10 +4751,10 @@
       <c r="BA45" s="41"/>
     </row>
     <row r="46" spans="1:53">
-      <c r="A46" s="110"/>
-      <c r="B46" s="113"/>
-      <c r="C46" s="113"/>
-      <c r="D46" s="98"/>
+      <c r="A46" s="128"/>
+      <c r="B46" s="120"/>
+      <c r="C46" s="120"/>
+      <c r="D46" s="134"/>
       <c r="E46" s="77" t="s">
         <v>81</v>
       </c>
@@ -4748,13 +4772,13 @@
       <c r="P46" s="39"/>
       <c r="Q46" s="45"/>
       <c r="R46" s="46"/>
-      <c r="S46" s="127"/>
-      <c r="T46" s="127"/>
-      <c r="U46" s="127"/>
-      <c r="V46" s="127"/>
-      <c r="W46" s="127"/>
-      <c r="X46" s="127"/>
-      <c r="Y46" s="127"/>
+      <c r="S46" s="97"/>
+      <c r="T46" s="97"/>
+      <c r="U46" s="97"/>
+      <c r="V46" s="97"/>
+      <c r="W46" s="97"/>
+      <c r="X46" s="97"/>
+      <c r="Y46" s="97"/>
       <c r="Z46" s="38"/>
       <c r="AA46" s="39"/>
       <c r="AB46" s="39"/>
@@ -4785,10 +4809,10 @@
       <c r="BA46" s="41"/>
     </row>
     <row r="47" spans="1:53">
-      <c r="A47" s="110"/>
-      <c r="B47" s="113"/>
-      <c r="C47" s="114"/>
-      <c r="D47" s="99"/>
+      <c r="A47" s="128"/>
+      <c r="B47" s="120"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="135"/>
       <c r="E47" s="76" t="s">
         <v>82</v>
       </c>
@@ -4806,13 +4830,13 @@
       <c r="P47" s="39"/>
       <c r="Q47" s="45"/>
       <c r="R47" s="46"/>
-      <c r="S47" s="127"/>
-      <c r="T47" s="127"/>
-      <c r="U47" s="127"/>
-      <c r="V47" s="127"/>
-      <c r="W47" s="127"/>
-      <c r="X47" s="127"/>
-      <c r="Y47" s="127"/>
+      <c r="S47" s="97"/>
+      <c r="T47" s="97"/>
+      <c r="U47" s="97"/>
+      <c r="V47" s="97"/>
+      <c r="W47" s="97"/>
+      <c r="X47" s="97"/>
+      <c r="Y47" s="97"/>
       <c r="Z47" s="38"/>
       <c r="AA47" s="39"/>
       <c r="AB47" s="39"/>
@@ -4843,12 +4867,12 @@
       <c r="BA47" s="41"/>
     </row>
     <row r="48" spans="1:53">
-      <c r="A48" s="110"/>
-      <c r="B48" s="113"/>
-      <c r="C48" s="112" t="s">
+      <c r="A48" s="128"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="97">
+      <c r="D48" s="133">
         <v>26</v>
       </c>
       <c r="E48" s="75" t="s">
@@ -4868,13 +4892,13 @@
       <c r="P48" s="39"/>
       <c r="Q48" s="45"/>
       <c r="R48" s="46"/>
-      <c r="S48" s="127"/>
-      <c r="T48" s="127"/>
-      <c r="U48" s="127"/>
-      <c r="V48" s="127"/>
-      <c r="W48" s="127"/>
-      <c r="X48" s="127"/>
-      <c r="Y48" s="127"/>
+      <c r="S48" s="97"/>
+      <c r="T48" s="97"/>
+      <c r="U48" s="97"/>
+      <c r="V48" s="97"/>
+      <c r="W48" s="97"/>
+      <c r="X48" s="97"/>
+      <c r="Y48" s="97"/>
       <c r="Z48" s="38"/>
       <c r="AA48" s="39"/>
       <c r="AB48" s="39"/>
@@ -4905,10 +4929,10 @@
       <c r="BA48" s="41"/>
     </row>
     <row r="49" spans="1:53">
-      <c r="A49" s="110"/>
-      <c r="B49" s="114"/>
-      <c r="C49" s="114"/>
-      <c r="D49" s="99"/>
+      <c r="A49" s="128"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="121"/>
+      <c r="D49" s="135"/>
       <c r="E49" s="76" t="s">
         <v>84</v>
       </c>
@@ -4926,13 +4950,13 @@
       <c r="P49" s="39"/>
       <c r="Q49" s="45"/>
       <c r="R49" s="46"/>
-      <c r="S49" s="127"/>
-      <c r="T49" s="127"/>
-      <c r="U49" s="127"/>
-      <c r="V49" s="127"/>
-      <c r="W49" s="127"/>
-      <c r="X49" s="127"/>
-      <c r="Y49" s="127"/>
+      <c r="S49" s="97"/>
+      <c r="T49" s="97"/>
+      <c r="U49" s="97"/>
+      <c r="V49" s="97"/>
+      <c r="W49" s="97"/>
+      <c r="X49" s="97"/>
+      <c r="Y49" s="97"/>
       <c r="Z49" s="38"/>
       <c r="AA49" s="39"/>
       <c r="AB49" s="39"/>
@@ -4963,8 +4987,8 @@
       <c r="BA49" s="41"/>
     </row>
     <row r="50" spans="1:53">
-      <c r="A50" s="110"/>
-      <c r="B50" s="112" t="s">
+      <c r="A50" s="128"/>
+      <c r="B50" s="119" t="s">
         <v>86</v>
       </c>
       <c r="C50" s="60" t="s">
@@ -4997,15 +5021,15 @@
       <c r="W50" s="39"/>
       <c r="X50" s="51"/>
       <c r="Y50" s="51"/>
-      <c r="Z50" s="128" t="s">
+      <c r="Z50" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="AA50" s="129"/>
-      <c r="AB50" s="129"/>
-      <c r="AC50" s="129"/>
-      <c r="AD50" s="129"/>
-      <c r="AE50" s="129"/>
-      <c r="AF50" s="130"/>
+      <c r="AA50" s="104"/>
+      <c r="AB50" s="104"/>
+      <c r="AC50" s="104"/>
+      <c r="AD50" s="104"/>
+      <c r="AE50" s="104"/>
+      <c r="AF50" s="105"/>
       <c r="AG50" s="51"/>
       <c r="AH50" s="51"/>
       <c r="AI50" s="51"/>
@@ -5029,8 +5053,8 @@
       <c r="BA50" s="41"/>
     </row>
     <row r="51" spans="1:53">
-      <c r="A51" s="110"/>
-      <c r="B51" s="113"/>
+      <c r="A51" s="128"/>
+      <c r="B51" s="120"/>
       <c r="C51" s="59" t="s">
         <v>89</v>
       </c>
@@ -5061,13 +5085,13 @@
       <c r="W51" s="39"/>
       <c r="X51" s="51"/>
       <c r="Y51" s="51"/>
-      <c r="Z51" s="131"/>
-      <c r="AA51" s="127"/>
-      <c r="AB51" s="127"/>
-      <c r="AC51" s="127"/>
-      <c r="AD51" s="127"/>
-      <c r="AE51" s="127"/>
-      <c r="AF51" s="132"/>
+      <c r="Z51" s="98"/>
+      <c r="AA51" s="97"/>
+      <c r="AB51" s="97"/>
+      <c r="AC51" s="97"/>
+      <c r="AD51" s="97"/>
+      <c r="AE51" s="97"/>
+      <c r="AF51" s="99"/>
       <c r="AG51" s="51"/>
       <c r="AH51" s="51"/>
       <c r="AI51" s="51"/>
@@ -5091,14 +5115,14 @@
       <c r="BA51" s="41"/>
     </row>
     <row r="52" spans="1:53">
-      <c r="A52" s="110"/>
-      <c r="B52" s="115" t="s">
+      <c r="A52" s="128"/>
+      <c r="B52" s="125" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="115" t="s">
+      <c r="C52" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="D52" s="100">
+      <c r="D52" s="131">
         <v>29</v>
       </c>
       <c r="E52" s="74" t="s">
@@ -5125,13 +5149,13 @@
       <c r="W52" s="39"/>
       <c r="X52" s="51"/>
       <c r="Y52" s="51"/>
-      <c r="Z52" s="131"/>
-      <c r="AA52" s="127"/>
-      <c r="AB52" s="127"/>
-      <c r="AC52" s="127"/>
-      <c r="AD52" s="127"/>
-      <c r="AE52" s="127"/>
-      <c r="AF52" s="132"/>
+      <c r="Z52" s="98"/>
+      <c r="AA52" s="97"/>
+      <c r="AB52" s="97"/>
+      <c r="AC52" s="97"/>
+      <c r="AD52" s="97"/>
+      <c r="AE52" s="97"/>
+      <c r="AF52" s="99"/>
       <c r="AG52" s="51"/>
       <c r="AH52" s="51"/>
       <c r="AI52" s="51"/>
@@ -5155,10 +5179,10 @@
       <c r="BA52" s="41"/>
     </row>
     <row r="53" spans="1:53">
-      <c r="A53" s="110"/>
-      <c r="B53" s="115"/>
-      <c r="C53" s="115"/>
-      <c r="D53" s="101"/>
+      <c r="A53" s="128"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="125"/>
+      <c r="D53" s="132"/>
       <c r="E53" s="31" t="s">
         <v>64</v>
       </c>
@@ -5183,13 +5207,13 @@
       <c r="W53" s="39"/>
       <c r="X53" s="51"/>
       <c r="Y53" s="51"/>
-      <c r="Z53" s="131"/>
-      <c r="AA53" s="127"/>
-      <c r="AB53" s="127"/>
-      <c r="AC53" s="127"/>
-      <c r="AD53" s="127"/>
-      <c r="AE53" s="127"/>
-      <c r="AF53" s="132"/>
+      <c r="Z53" s="98"/>
+      <c r="AA53" s="97"/>
+      <c r="AB53" s="97"/>
+      <c r="AC53" s="97"/>
+      <c r="AD53" s="97"/>
+      <c r="AE53" s="97"/>
+      <c r="AF53" s="99"/>
       <c r="AG53" s="51"/>
       <c r="AH53" s="51"/>
       <c r="AI53" s="51"/>
@@ -5213,8 +5237,8 @@
       <c r="BA53" s="41"/>
     </row>
     <row r="54" spans="1:53">
-      <c r="A54" s="110"/>
-      <c r="B54" s="108" t="s">
+      <c r="A54" s="128"/>
+      <c r="B54" s="126" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="31" t="s">
@@ -5248,13 +5272,13 @@
       <c r="W54" s="39"/>
       <c r="X54" s="51"/>
       <c r="Y54" s="51"/>
-      <c r="Z54" s="131"/>
-      <c r="AA54" s="127"/>
-      <c r="AB54" s="127"/>
-      <c r="AC54" s="127"/>
-      <c r="AD54" s="127"/>
-      <c r="AE54" s="127"/>
-      <c r="AF54" s="132"/>
+      <c r="Z54" s="98"/>
+      <c r="AA54" s="97"/>
+      <c r="AB54" s="97"/>
+      <c r="AC54" s="97"/>
+      <c r="AD54" s="97"/>
+      <c r="AE54" s="97"/>
+      <c r="AF54" s="99"/>
       <c r="AG54" s="51"/>
       <c r="AH54" s="51"/>
       <c r="AI54" s="51"/>
@@ -5278,8 +5302,8 @@
       <c r="BA54" s="41"/>
     </row>
     <row r="55" spans="1:53">
-      <c r="A55" s="111"/>
-      <c r="B55" s="108"/>
+      <c r="A55" s="129"/>
+      <c r="B55" s="126"/>
       <c r="C55" s="31" t="s">
         <v>96</v>
       </c>
@@ -5310,13 +5334,13 @@
       <c r="W55" s="39"/>
       <c r="X55" s="51"/>
       <c r="Y55" s="51"/>
-      <c r="Z55" s="131"/>
-      <c r="AA55" s="127"/>
-      <c r="AB55" s="127"/>
-      <c r="AC55" s="127"/>
-      <c r="AD55" s="127"/>
-      <c r="AE55" s="127"/>
-      <c r="AF55" s="132"/>
+      <c r="Z55" s="98"/>
+      <c r="AA55" s="97"/>
+      <c r="AB55" s="97"/>
+      <c r="AC55" s="97"/>
+      <c r="AD55" s="97"/>
+      <c r="AE55" s="97"/>
+      <c r="AF55" s="99"/>
       <c r="AG55" s="51"/>
       <c r="AH55" s="51"/>
       <c r="AI55" s="51"/>
@@ -5345,29 +5369,26 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="S42:Y42"/>
-    <mergeCell ref="Z50:AF50"/>
-    <mergeCell ref="Z28:AF28"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A31"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A45:A55"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C35:C36"/>
@@ -5377,19 +5398,30 @@
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A3:A31"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="S42:Y42"/>
+    <mergeCell ref="Z50:AF50"/>
+    <mergeCell ref="Z28:AF28"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C39:C41"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="D11:D12"/>
@@ -5399,14 +5431,6 @@
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>